<commit_message>
updated TEA input template to fix the bug about taxing negative income
</commit_message>
<xml_diff>
--- a/TEA_user_input_Dec.29 sim results_template.xlsx
+++ b/TEA_user_input_Dec.29 sim results_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Qingshi/Documents/University of British Columbia/Publications_QT/Published_journal/[Jason] electrocatalysis LCA/LA project/python scripts/upload to github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtu2020\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591E8654-97D9-1C45-95DE-0657F452065E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4E018C-2C4E-4B8D-AAC6-54CDA02E688F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -38,14 +38,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -780,7 +772,7 @@
     <numFmt numFmtId="168" formatCode="0.00000"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1691,13 +1683,13 @@
       <selection activeCell="E17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="15.19921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.796875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="36.6">
       <c r="B1" s="36" t="s">
         <v>29</v>
       </c>
@@ -1708,7 +1700,7 @@
       <c r="G1" s="37"/>
       <c r="H1" s="37"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
@@ -1719,7 +1711,7 @@
       <c r="N3" s="38"/>
       <c r="O3" s="38"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="B4" s="14" t="s">
         <v>118</v>
       </c>
@@ -1727,13 +1719,13 @@
       <c r="N4" s="38"/>
       <c r="O4" s="38"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="B5" s="16"/>
       <c r="M5" s="38"/>
       <c r="N5" s="38"/>
       <c r="O5" s="38"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" s="15" t="s">
         <v>37</v>
       </c>
@@ -1741,33 +1733,33 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15">
       <c r="A7" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" s="15"/>
       <c r="B8" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="B10" s="14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="B12" s="14" t="s">
         <v>39</v>
       </c>
@@ -1788,18 +1780,18 @@
       <selection activeCell="E1" sqref="E1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1814,7 +1806,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1823,13 +1815,13 @@
       </c>
       <c r="C3" s="58">
         <f>Intermediate!B55</f>
-        <v>-3603802.5330074122</v>
+        <v>-4553308.4754070779</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1844,7 +1836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1859,16 +1851,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="60" t="e">
         <f>Intermediate!B56*100</f>
-        <v>-13.026556612865347</v>
+        <v>#NUM!</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1886,26 +1878,26 @@
   </sheetPr>
   <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="V50" sqref="V50"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="55.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="8"/>
-    <col min="4" max="4" width="17.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="21" width="10.83203125" style="8"/>
-    <col min="22" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="55.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="8"/>
+    <col min="4" max="4" width="17.296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="21" width="10.796875" style="8"/>
+    <col min="22" max="16384" width="10.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21">
       <c r="A1" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="B2" s="6" t="s">
         <v>66</v>
       </c>
@@ -1913,7 +1905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>110</v>
       </c>
@@ -1925,7 +1917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
         <v>111</v>
       </c>
@@ -1937,7 +1929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="20" t="s">
         <v>112</v>
       </c>
@@ -1949,12 +1941,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="21">
       <c r="A7" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" s="6" t="s">
         <v>66</v>
@@ -1963,7 +1955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="47" t="s">
         <v>89</v>
       </c>
@@ -1975,7 +1967,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="47" t="s">
         <v>96</v>
       </c>
@@ -1987,7 +1979,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="48" t="s">
         <v>36</v>
       </c>
@@ -1999,12 +1991,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="21">
       <c r="A13" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="29"/>
       <c r="B14" s="8" t="s">
         <v>87</v>
@@ -2025,7 +2017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="6" t="str">
         <f>Electrocatalysis!A4</f>
         <v>Glycerine</v>
@@ -2053,7 +2045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="6" t="str">
         <f>Electrocatalysis!A5</f>
         <v>Lime</v>
@@ -2081,7 +2073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="6" t="str">
         <f>Electrocatalysis!A6</f>
         <v>Methanol</v>
@@ -2109,7 +2101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="str">
         <f>Electrocatalysis!A7</f>
         <v>Sodium hydroxide</v>
@@ -2137,7 +2129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="6" t="str">
         <f>Electrocatalysis!A8</f>
         <v>Sulfuric acid</v>
@@ -2165,7 +2157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="6" t="str">
         <f>Electrocatalysis!A9</f>
         <v>Water</v>
@@ -2193,7 +2185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="6" t="str">
         <f>Electrocatalysis!A10</f>
         <v>Cooling water (refrigerated)</v>
@@ -2221,7 +2213,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="6" t="str">
         <f>Electrocatalysis!A11</f>
         <v>Heat, from steam</v>
@@ -2249,7 +2241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="6" t="str">
         <f>Electrocatalysis!A12</f>
         <v>Electricity</v>
@@ -2277,7 +2269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="6" t="str">
         <f>Electrocatalysis!A13</f>
         <v>Lactic acid</v>
@@ -2305,7 +2297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="6" t="str">
         <f>Electrocatalysis!A14</f>
         <v>Glycolic acid</v>
@@ -2333,7 +2325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="6" t="str">
         <f>Electrocatalysis!A15</f>
         <v>Glyceric acid</v>
@@ -2361,7 +2353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="6" t="str">
         <f>Electrocatalysis!A16</f>
         <v>Oxalic acid</v>
@@ -2389,7 +2381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="6" t="str">
         <f>Electrocatalysis!A17</f>
         <v>Formic acid</v>
@@ -2417,7 +2409,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="6" t="str">
         <f>Electrocatalysis!A18</f>
         <v>Hazardous waste, for incineration</v>
@@ -2445,12 +2437,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="21">
       <c r="A31" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="B32" s="8" t="s">
         <v>88</v>
       </c>
@@ -2458,7 +2450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22">
       <c r="A33" s="6" t="s">
         <v>105</v>
       </c>
@@ -2470,7 +2462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22">
       <c r="A34" s="6" t="s">
         <v>92</v>
       </c>
@@ -2482,7 +2474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22">
       <c r="A35" s="6" t="s">
         <v>106</v>
       </c>
@@ -2494,7 +2486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22">
       <c r="A36" s="20" t="s">
         <v>86</v>
       </c>
@@ -2506,7 +2498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22">
       <c r="A37" s="20" t="s">
         <v>95</v>
       </c>
@@ -2518,7 +2510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22">
       <c r="A38" s="35" t="s">
         <v>11</v>
       </c>
@@ -2530,12 +2522,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="21">
       <c r="A40" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" s="33" customFormat="1">
       <c r="A41" s="29"/>
       <c r="B41" s="6" t="s">
         <v>66</v>
@@ -2562,7 +2554,7 @@
       <c r="T41" s="32"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22">
       <c r="A42" s="4" t="s">
         <v>100</v>
       </c>
@@ -2574,7 +2566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22">
       <c r="A43" s="4" t="s">
         <v>104</v>
       </c>
@@ -2586,7 +2578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22">
       <c r="A44" s="4" t="s">
         <v>101</v>
       </c>
@@ -2598,7 +2590,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22">
       <c r="A45" s="31" t="s">
         <v>102</v>
       </c>
@@ -2610,15 +2602,15 @@
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22">
       <c r="A46" s="48"/>
     </row>
-    <row r="47" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" ht="21">
       <c r="A47" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22">
       <c r="A48" s="5"/>
       <c r="B48" s="8">
         <v>0</v>
@@ -2684,7 +2676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:22">
       <c r="A49" s="7" t="s">
         <v>152</v>
       </c>
@@ -2770,93 +2762,93 @@
         <v>-118499.12265398791</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22">
       <c r="A50" s="46" t="s">
         <v>153</v>
       </c>
       <c r="B50" s="59"/>
       <c r="C50" s="8">
-        <f>C49*(1-'Financial param'!$I$10/100)</f>
-        <v>-274904.46597509214</v>
+        <f>IF(C49&gt;0,C49*(1-'Financial param'!$I$10/100),C49)</f>
+        <v>-422929.94765398791</v>
       </c>
       <c r="D50" s="8">
-        <f>D49*(1-'Financial param'!$I$10/100)</f>
-        <v>-264489.72722509218</v>
+        <f>IF(D49&gt;0,D49*(1-'Financial param'!$I$10/100),D49)</f>
+        <v>-406907.27265398792</v>
       </c>
       <c r="E50" s="8">
-        <f>E49*(1-'Financial param'!$I$10/100)</f>
-        <v>-254074.98847509216</v>
+        <f>IF(E49&gt;0,E49*(1-'Financial param'!$I$10/100),E49)</f>
+        <v>-390884.59765398793</v>
       </c>
       <c r="F50" s="8">
-        <f>F49*(1-'Financial param'!$I$10/100)</f>
-        <v>-243660.24972509217</v>
+        <f>IF(F49&gt;0,F49*(1-'Financial param'!$I$10/100),F49)</f>
+        <v>-374861.92265398795</v>
       </c>
       <c r="G50" s="8">
-        <f>G49*(1-'Financial param'!$I$10/100)</f>
-        <v>-233245.51097509218</v>
+        <f>IF(G49&gt;0,G49*(1-'Financial param'!$I$10/100),G49)</f>
+        <v>-358839.24765398796</v>
       </c>
       <c r="H50" s="8">
-        <f>H49*(1-'Financial param'!$I$10/100)</f>
-        <v>-222830.77222509214</v>
+        <f>IF(H49&gt;0,H49*(1-'Financial param'!$I$10/100),H49)</f>
+        <v>-342816.57265398791</v>
       </c>
       <c r="I50" s="8">
-        <f>I49*(1-'Financial param'!$I$10/100)</f>
-        <v>-212416.03347509215</v>
+        <f>IF(I49&gt;0,I49*(1-'Financial param'!$I$10/100),I49)</f>
+        <v>-326793.89765398792</v>
       </c>
       <c r="J50" s="8">
-        <f>J49*(1-'Financial param'!$I$10/100)</f>
-        <v>-202001.29472509216</v>
+        <f>IF(J49&gt;0,J49*(1-'Financial param'!$I$10/100),J49)</f>
+        <v>-310771.22265398793</v>
       </c>
       <c r="K50" s="8">
-        <f>K49*(1-'Financial param'!$I$10/100)</f>
-        <v>-191586.55597509214</v>
+        <f>IF(K49&gt;0,K49*(1-'Financial param'!$I$10/100),K49)</f>
+        <v>-294748.54765398789</v>
       </c>
       <c r="L50" s="8">
-        <f>L49*(1-'Financial param'!$I$10/100)</f>
-        <v>-181171.81722509218</v>
+        <f>IF(L49&gt;0,L49*(1-'Financial param'!$I$10/100),L49)</f>
+        <v>-278725.87265398796</v>
       </c>
       <c r="M50" s="8">
-        <f>M49*(1-'Financial param'!$I$10/100)</f>
-        <v>-170757.07847509216</v>
+        <f>IF(M49&gt;0,M49*(1-'Financial param'!$I$10/100),M49)</f>
+        <v>-262703.19765398791</v>
       </c>
       <c r="N50" s="8">
-        <f>N49*(1-'Financial param'!$I$10/100)</f>
-        <v>-160342.33972509214</v>
+        <f>IF(N49&gt;0,N49*(1-'Financial param'!$I$10/100),N49)</f>
+        <v>-246680.52265398792</v>
       </c>
       <c r="O50" s="8">
-        <f>O49*(1-'Financial param'!$I$10/100)</f>
-        <v>-149927.60097509215</v>
+        <f>IF(O49&gt;0,O49*(1-'Financial param'!$I$10/100),O49)</f>
+        <v>-230657.84765398793</v>
       </c>
       <c r="P50" s="8">
-        <f>P49*(1-'Financial param'!$I$10/100)</f>
-        <v>-139512.86222509216</v>
+        <f>IF(P49&gt;0,P49*(1-'Financial param'!$I$10/100),P49)</f>
+        <v>-214635.17265398792</v>
       </c>
       <c r="Q50" s="8">
-        <f>Q49*(1-'Financial param'!$I$10/100)</f>
-        <v>-129098.12347509214</v>
+        <f>IF(Q49&gt;0,Q49*(1-'Financial param'!$I$10/100),Q49)</f>
+        <v>-198612.4976539879</v>
       </c>
       <c r="R50" s="8">
-        <f>R49*(1-'Financial param'!$I$10/100)</f>
-        <v>-118683.38472509214</v>
+        <f>IF(R49&gt;0,R49*(1-'Financial param'!$I$10/100),R49)</f>
+        <v>-182589.82265398791</v>
       </c>
       <c r="S50" s="8">
-        <f>S49*(1-'Financial param'!$I$10/100)</f>
-        <v>-108268.64597509215</v>
+        <f>IF(S49&gt;0,S49*(1-'Financial param'!$I$10/100),S49)</f>
+        <v>-166567.14765398792</v>
       </c>
       <c r="T50" s="8">
-        <f>T49*(1-'Financial param'!$I$10/100)</f>
-        <v>-97853.907225092145</v>
+        <f>IF(T49&gt;0,T49*(1-'Financial param'!$I$10/100),T49)</f>
+        <v>-150544.4726539879</v>
       </c>
       <c r="U50" s="8">
-        <f>U49*(1-'Financial param'!$I$10/100)</f>
-        <v>-87439.168475092156</v>
+        <f>IF(U49&gt;0,U49*(1-'Financial param'!$I$10/100),U49)</f>
+        <v>-134521.79765398792</v>
       </c>
       <c r="V50" s="8">
-        <f>V49*(1-'Financial param'!$I$10/100)</f>
-        <v>-77024.429725092152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+        <f>IF(V49&gt;0,V49*(1-'Financial param'!$I$10/100),V49)</f>
+        <v>-118499.12265398791</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22">
       <c r="A51" s="27" t="s">
         <v>151</v>
       </c>
@@ -2866,86 +2858,86 @@
       </c>
       <c r="C51" s="8">
         <f>C50+$B$42+$B$43</f>
-        <v>-114677.71597509214</v>
+        <v>-262703.19765398791</v>
       </c>
       <c r="D51" s="8">
         <f t="shared" ref="D51:V51" si="0">D50+$B$42+$B$43</f>
-        <v>-104262.97722509218</v>
+        <v>-246680.52265398792</v>
       </c>
       <c r="E51" s="8">
         <f t="shared" si="0"/>
-        <v>-93848.238475092163</v>
+        <v>-230657.84765398793</v>
       </c>
       <c r="F51" s="8">
         <f t="shared" si="0"/>
-        <v>-83433.499725092173</v>
+        <v>-214635.17265398795</v>
       </c>
       <c r="G51" s="8">
         <f t="shared" si="0"/>
-        <v>-73018.760975092184</v>
+        <v>-198612.49765398796</v>
       </c>
       <c r="H51" s="8">
         <f t="shared" si="0"/>
-        <v>-62604.022225092136</v>
+        <v>-182589.82265398791</v>
       </c>
       <c r="I51" s="8">
         <f t="shared" si="0"/>
-        <v>-52189.283475092147</v>
+        <v>-166567.14765398792</v>
       </c>
       <c r="J51" s="8">
         <f t="shared" si="0"/>
-        <v>-41774.544725092157</v>
+        <v>-150544.47265398793</v>
       </c>
       <c r="K51" s="8">
         <f t="shared" si="0"/>
-        <v>-31359.805975092138</v>
+        <v>-134521.79765398789</v>
       </c>
       <c r="L51" s="8">
         <f t="shared" si="0"/>
-        <v>-20945.067225092178</v>
+        <v>-118499.12265398796</v>
       </c>
       <c r="M51" s="8">
         <f t="shared" si="0"/>
-        <v>-10530.328475092159</v>
+        <v>-102476.44765398791</v>
       </c>
       <c r="N51" s="8">
         <f t="shared" si="0"/>
-        <v>-115.58972509214072</v>
+        <v>-86453.772653987922</v>
       </c>
       <c r="O51" s="8">
         <f t="shared" si="0"/>
-        <v>10299.149024907849</v>
+        <v>-70431.097653987934</v>
       </c>
       <c r="P51" s="8">
         <f t="shared" si="0"/>
-        <v>20713.887774907838</v>
+        <v>-54408.422653987916</v>
       </c>
       <c r="Q51" s="8">
         <f t="shared" si="0"/>
-        <v>31128.626524907857</v>
+        <v>-38385.747653987899</v>
       </c>
       <c r="R51" s="8">
         <f t="shared" si="0"/>
-        <v>41543.365274907861</v>
+        <v>-22363.072653987911</v>
       </c>
       <c r="S51" s="8">
         <f>S50+$B$42+$B$43</f>
-        <v>51958.104024907851</v>
+        <v>-6340.3976539879222</v>
       </c>
       <c r="T51" s="8">
         <f t="shared" si="0"/>
-        <v>62372.842774907855</v>
+        <v>9682.2773460120952</v>
       </c>
       <c r="U51" s="8">
         <f t="shared" si="0"/>
-        <v>72787.581524907844</v>
+        <v>25704.952346012084</v>
       </c>
       <c r="V51" s="8">
         <f t="shared" si="0"/>
-        <v>83202.320274907848</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+        <v>41727.627346012086</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
       <c r="A52" s="27" t="s">
         <v>158</v>
       </c>
@@ -2955,86 +2947,86 @@
       </c>
       <c r="C52" s="8">
         <f>C51/((1+'Financial param'!$I$4/100)^Intermediate!C48)</f>
-        <v>-104252.46906826558</v>
+        <v>-238821.08877635264</v>
       </c>
       <c r="D52" s="8">
         <f>D51/((1+'Financial param'!$I$4/100)^Intermediate!D48)</f>
-        <v>-86167.749772803436</v>
+        <v>-203868.20054048585</v>
       </c>
       <c r="E52" s="8">
         <f>E51/((1+'Financial param'!$I$4/100)^Intermediate!E48)</f>
-        <v>-70509.570604877634</v>
+        <v>-173296.65488654235</v>
       </c>
       <c r="F52" s="8">
         <f>F51/((1+'Financial param'!$I$4/100)^Intermediate!F48)</f>
-        <v>-56986.202940435862</v>
+        <v>-146598.7109172788</v>
       </c>
       <c r="G52" s="8">
         <f>G51/((1+'Financial param'!$I$4/100)^Intermediate!G48)</f>
-        <v>-45338.905672794433</v>
+        <v>-123322.73481939752</v>
       </c>
       <c r="H52" s="8">
         <f>H51/((1+'Financial param'!$I$4/100)^Intermediate!H48)</f>
-        <v>-35338.338462571766</v>
+        <v>-103067.19478131874</v>
       </c>
       <c r="I52" s="8">
         <f>I51/((1+'Financial param'!$I$4/100)^Intermediate!I48)</f>
-        <v>-26781.354499887191</v>
+        <v>-85475.284049176669</v>
       </c>
       <c r="J52" s="8">
         <f>J51/((1+'Financial param'!$I$4/100)^Intermediate!J48)</f>
-        <v>-19488.133419157071</v>
+        <v>-70230.107542867729</v>
       </c>
       <c r="K52" s="8">
         <f>K51/((1+'Financial param'!$I$4/100)^Intermediate!K48)</f>
-        <v>-13299.61902665979</v>
+        <v>-57050.374004241559</v>
       </c>
       <c r="L52" s="8">
         <f>L51/((1+'Financial param'!$I$4/100)^Intermediate!L48)</f>
-        <v>-8075.2301152847067</v>
+        <v>-45686.541542532032</v>
       </c>
       <c r="M52" s="8">
         <f>M51/((1+'Financial param'!$I$4/100)^Intermediate!M48)</f>
-        <v>-3690.8158900549934</v>
+        <v>-35917.369743246985</v>
       </c>
       <c r="N52" s="8">
         <f>N51/((1+'Financial param'!$I$4/100)^Intermediate!N48)</f>
-        <v>-36.830448625024118</v>
+        <v>-27546.836274885434</v>
       </c>
       <c r="O52" s="8">
         <f>O51/((1+'Financial param'!$I$4/100)^Intermediate!O48)</f>
-        <v>2983.2966141156448</v>
+        <v>-20401.3802161165</v>
       </c>
       <c r="P52" s="8">
         <f>P51/((1+'Financial param'!$I$4/100)^Intermediate!P48)</f>
-        <v>5454.6140493218518</v>
+        <v>-14327.438182289961</v>
       </c>
       <c r="Q52" s="8">
         <f>Q51/((1+'Financial param'!$I$4/100)^Intermediate!Q48)</f>
-        <v>7451.9456978449907</v>
+        <v>-9189.2427974557195</v>
       </c>
       <c r="R52" s="8">
         <f>R51/((1+'Financial param'!$I$4/100)^Intermediate!R48)</f>
-        <v>9041.0466825926651</v>
+        <v>-4866.856175299692</v>
       </c>
       <c r="S52" s="8">
         <f>S51/((1+'Financial param'!$I$4/100)^Intermediate!S48)</f>
-        <v>10279.633887486667</v>
+        <v>-1254.4138745484333</v>
       </c>
       <c r="T52" s="8">
         <f>T51/((1+'Financial param'!$I$4/100)^Intermediate!T48)</f>
-        <v>11218.304024692567</v>
+        <v>1741.4426870191282</v>
       </c>
       <c r="U52" s="8">
         <f>U51/((1+'Financial param'!$I$4/100)^Intermediate!U48)</f>
-        <v>11901.351212261961</v>
+        <v>4202.9651123888498</v>
       </c>
       <c r="V52" s="8">
         <f>V51/((1+'Financial param'!$I$4/100)^Intermediate!V48)</f>
-        <v>12367.494745689053</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+        <v>6202.5459175506985</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
       <c r="A53" s="46" t="s">
         <v>155</v>
       </c>
@@ -3120,29 +3112,29 @@
         <v>-352103.42499999999</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22">
       <c r="A54" s="52"/>
       <c r="B54" s="53"/>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22">
       <c r="A55" s="34" t="s">
         <v>150</v>
       </c>
       <c r="B55" s="44">
         <f>NPV('Financial param'!I4/100,Intermediate!C51:V51)+B51</f>
-        <v>-3603802.5330074122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+        <v>-4553308.4754070779</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="B56" s="66">
+      <c r="B56" s="66" t="e">
         <f>IRR(B51:V51)</f>
-        <v>-0.13026556612865348</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" s="54" t="s">
         <v>156</v>
       </c>
@@ -3227,48 +3219,48 @@
         <v>2.8019303048922315</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22">
       <c r="A58" s="28"/>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22">
       <c r="A59" s="28"/>
     </row>
-    <row r="60" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="21">
       <c r="A60" s="28"/>
       <c r="C60" s="50"/>
       <c r="D60" s="51"/>
       <c r="E60" s="50"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="21">
       <c r="A61" s="28"/>
       <c r="C61" s="50"/>
       <c r="D61" s="50"/>
       <c r="E61" s="50"/>
       <c r="F61" s="50"/>
     </row>
-    <row r="62" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" ht="21">
       <c r="A62" s="28"/>
       <c r="C62" s="50"/>
       <c r="D62" s="50"/>
       <c r="E62" s="50"/>
       <c r="F62" s="50"/>
     </row>
-    <row r="63" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="21">
       <c r="A63" s="28"/>
       <c r="C63" s="50"/>
       <c r="D63" s="50"/>
       <c r="E63" s="50"/>
       <c r="F63" s="50"/>
     </row>
-    <row r="64" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="21">
       <c r="A64" s="28"/>
       <c r="C64" s="50"/>
       <c r="D64" s="50"/>
       <c r="E64" s="50"/>
       <c r="F64" s="50"/>
     </row>
-    <row r="65" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="21">
       <c r="A65" s="28"/>
       <c r="C65" s="50"/>
       <c r="D65" s="50"/>
@@ -3286,19 +3278,19 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.69921875" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="21">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -3306,7 +3298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3338,7 +3330,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3364,7 +3356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="G4">
         <v>1</v>
       </c>
@@ -3378,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="G5">
         <v>2</v>
       </c>
@@ -3392,7 +3384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="G6">
         <v>3</v>
       </c>
@@ -3406,7 +3398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="G7">
         <v>4</v>
       </c>
@@ -3420,7 +3412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="G8">
         <v>5</v>
       </c>
@@ -3434,7 +3426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="G9">
         <v>6</v>
       </c>
@@ -3448,7 +3440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="G10">
         <v>7</v>
       </c>
@@ -3462,7 +3454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="G11">
         <v>8</v>
       </c>
@@ -3490,20 +3482,20 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="21">
       <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3521,7 +3513,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -3537,7 +3529,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="41"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3551,7 +3543,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3565,7 +3557,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3579,7 +3571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="B7" s="43"/>
     </row>
   </sheetData>
@@ -3595,21 +3587,21 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21">
       <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3630,7 +3622,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3651,7 +3643,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3672,7 +3664,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3693,7 +3685,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3714,7 +3706,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3735,7 +3727,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>5</v>
       </c>
@@ -3756,7 +3748,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>6</v>
       </c>
@@ -3777,7 +3769,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>7</v>
       </c>
@@ -3798,7 +3790,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3819,7 +3811,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>9</v>
       </c>
@@ -3840,7 +3832,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>10</v>
       </c>
@@ -3861,7 +3853,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>11</v>
       </c>
@@ -3882,7 +3874,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>12</v>
       </c>
@@ -3903,7 +3895,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>13</v>
       </c>
@@ -3924,7 +3916,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>14</v>
       </c>
@@ -3945,7 +3937,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>15</v>
       </c>
@@ -3966,7 +3958,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>16</v>
       </c>
@@ -3987,7 +3979,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>17</v>
       </c>
@@ -4008,7 +4000,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>18</v>
       </c>
@@ -4044,15 +4036,15 @@
       <selection activeCell="B4" sqref="B4:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="67" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="121.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="22" t="s">
         <v>53</v>
       </c>
@@ -4060,7 +4052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="21">
       <c r="A2" s="22" t="s">
         <v>51</v>
       </c>
@@ -4068,7 +4060,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="11" customFormat="1" ht="42">
       <c r="A3" s="23" t="s">
         <v>62</v>
       </c>
@@ -4083,7 +4075,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="14" customFormat="1">
       <c r="A4" s="14" t="s">
         <v>43</v>
       </c>
@@ -4095,7 +4087,7 @@
       </c>
       <c r="E4" s="69"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -4106,7 +4098,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4117,7 +4109,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -4129,7 +4121,7 @@
       </c>
       <c r="E7" s="61"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -4141,7 +4133,7 @@
       </c>
       <c r="E8" s="65"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -4153,7 +4145,7 @@
       </c>
       <c r="E9" s="61"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -4165,7 +4157,7 @@
       </c>
       <c r="E10" s="61"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -4177,7 +4169,7 @@
       </c>
       <c r="E11" s="61"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -4189,7 +4181,7 @@
       </c>
       <c r="E12" s="61"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
         <v>52</v>
       </c>
@@ -4200,7 +4192,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4211,7 +4203,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4222,7 +4214,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -4233,7 +4225,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -4244,7 +4236,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -4269,14 +4261,14 @@
       <selection sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="67" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="22" t="s">
         <v>53</v>
       </c>
@@ -4284,7 +4276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="21">
       <c r="A2" s="22" t="s">
         <v>51</v>
       </c>
@@ -4292,7 +4284,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="11" customFormat="1" ht="42">
       <c r="A3" s="23" t="s">
         <v>62</v>
       </c>
@@ -4309,7 +4301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4320,7 +4312,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -4331,7 +4323,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4342,7 +4334,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -4353,7 +4345,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -4364,7 +4356,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -4375,7 +4367,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -4386,7 +4378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -4397,7 +4389,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -4408,7 +4400,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
         <v>52</v>
       </c>
@@ -4419,7 +4411,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4430,7 +4422,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4441,7 +4433,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -4452,7 +4444,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -4463,7 +4455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -4488,30 +4480,30 @@
       <selection activeCell="B3" sqref="B3:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.5" customWidth="1"/>
     <col min="13" max="13" width="34" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.69921875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="21">
       <c r="A1" s="21" t="s">
         <v>64</v>
       </c>
@@ -4531,7 +4523,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="20" t="s">
         <v>65</v>
       </c>
@@ -4595,7 +4587,7 @@
         <v>907.18499999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" t="str">
         <f>Electrocatalysis!A4</f>
         <v>Glycerine</v>
@@ -4640,7 +4632,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" t="str">
         <f>Electrocatalysis!A5</f>
         <v>Lime</v>
@@ -4675,7 +4667,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" t="str">
         <f>Electrocatalysis!A6</f>
         <v>Methanol</v>
@@ -4692,7 +4684,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24">
       <c r="A6" t="str">
         <f>Electrocatalysis!A7</f>
         <v>Sodium hydroxide</v>
@@ -4709,7 +4701,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="A7" t="str">
         <f>Electrocatalysis!A8</f>
         <v>Sulfuric acid</v>
@@ -4726,7 +4718,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24">
       <c r="A8" t="str">
         <f>Electrocatalysis!A9</f>
         <v>Water</v>
@@ -4743,7 +4735,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="A9" t="str">
         <f>Electrocatalysis!A10</f>
         <v>Cooling water (refrigerated)</v>
@@ -4760,7 +4752,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="A10" t="str">
         <f>Electrocatalysis!A11</f>
         <v>Heat, from steam</v>
@@ -4777,7 +4769,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" t="str">
         <f>Electrocatalysis!A12</f>
         <v>Electricity</v>
@@ -4794,7 +4786,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="A12" t="str">
         <f>Electrocatalysis!A13</f>
         <v>Lactic acid</v>
@@ -4811,7 +4803,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24">
       <c r="A13" t="str">
         <f>Electrocatalysis!A14</f>
         <v>Glycolic acid</v>
@@ -4827,7 +4819,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24">
       <c r="A14" t="str">
         <f>Electrocatalysis!A15</f>
         <v>Glyceric acid</v>
@@ -4847,7 +4839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24">
       <c r="A15" t="str">
         <f>Electrocatalysis!A16</f>
         <v>Oxalic acid</v>
@@ -4866,7 +4858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" t="str">
         <f>Electrocatalysis!A17</f>
         <v>Formic acid</v>
@@ -4880,7 +4872,7 @@
       </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="str">
         <f>Electrocatalysis!A18</f>
         <v>Hazardous waste, for incineration</v>

</xml_diff>